<commit_message>
Account Creation Page validation test.
</commit_message>
<xml_diff>
--- a/src/main/java/com/test/automation/uiAutomation/data/TestData.xlsx
+++ b/src/main/java/com/test/automation/uiAutomation/data/TestData.xlsx
@@ -5,14 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saurabhsharma/Automation_Workspace/UI_Automation/uiAutomation/src/main/java/com/test/automation/uiAutomation/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saurabhsharma/Automation_Workspace/UI_Automation/FirstClone/uiAutomationRepo/src/main/java/com/test/automation/uiAutomation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
+    <sheet name="AccountCreationData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="57">
   <si>
     <t>UserName</t>
   </si>
@@ -41,9 +42,6 @@
     <t>saurabhsharma81285@gmail.com</t>
   </si>
   <si>
-    <t>Pass123</t>
-  </si>
-  <si>
     <t>Sau97601@gmail.com</t>
   </si>
   <si>
@@ -66,6 +64,141 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>DayOfDOB</t>
+  </si>
+  <si>
+    <t>MonthOfDOB</t>
+  </si>
+  <si>
+    <t>FirstLineOfAddress</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>AddressAlias</t>
+  </si>
+  <si>
+    <t>MobileNumber</t>
+  </si>
+  <si>
+    <t>CountryName</t>
+  </si>
+  <si>
+    <t>StateName</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Saurabh</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>Shriya1@2015</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>5630 N Sheridan</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>FNU</t>
+  </si>
+  <si>
+    <t>Bharathi</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>Shriya</t>
+  </si>
+  <si>
+    <t>Gaurav</t>
+  </si>
+  <si>
+    <t>Vabhav</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>YearOfDOB</t>
+  </si>
+  <si>
+    <t>test124@gmail.com</t>
+  </si>
+  <si>
+    <t>pass567</t>
+  </si>
+  <si>
+    <t>"8"</t>
+  </si>
+  <si>
+    <t>"22"</t>
+  </si>
+  <si>
+    <t>"28"</t>
+  </si>
+  <si>
+    <t>"6"</t>
+  </si>
+  <si>
+    <t>"1985"</t>
+  </si>
+  <si>
+    <t>"1986"</t>
+  </si>
+  <si>
+    <t>"2015"</t>
+  </si>
+  <si>
+    <t>"1112223334"</t>
+  </si>
+  <si>
+    <t>"60661"</t>
+  </si>
+  <si>
+    <t>United States</t>
   </si>
 </sst>
 </file>
@@ -131,11 +264,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -414,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -441,43 +580,54 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -486,6 +636,340 @@
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
     <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="6"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="6"/>
+    <col min="9" max="9" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.5" style="7" customWidth="1"/>
+    <col min="15" max="15" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Couple of Hardcoded parameters are made dynamic.
</commit_message>
<xml_diff>
--- a/src/main/java/com/test/automation/uiAutomation/data/TestData.xlsx
+++ b/src/main/java/com/test/automation/uiAutomation/data/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="46">
   <si>
     <t>UserName</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Shriya1@2015</t>
   </si>
   <si>
-    <t>June</t>
-  </si>
-  <si>
     <t>5630 N Sheridan</t>
   </si>
   <si>
@@ -138,12 +135,6 @@
     <t>Bharathi</t>
   </si>
   <si>
-    <t>July</t>
-  </si>
-  <si>
-    <t>December</t>
-  </si>
-  <si>
     <t>male</t>
   </si>
   <si>
@@ -156,12 +147,6 @@
     <t>Vabhav</t>
   </si>
   <si>
-    <t>August</t>
-  </si>
-  <si>
-    <t>March</t>
-  </si>
-  <si>
     <t>YearOfDOB</t>
   </si>
   <si>
@@ -171,40 +156,26 @@
     <t>pass567</t>
   </si>
   <si>
-    <t>"8"</t>
-  </si>
-  <si>
-    <t>"22"</t>
-  </si>
-  <si>
-    <t>"28"</t>
-  </si>
-  <si>
-    <t>"6"</t>
-  </si>
-  <si>
-    <t>"1985"</t>
-  </si>
-  <si>
-    <t>"1986"</t>
-  </si>
-  <si>
-    <t>"2015"</t>
-  </si>
-  <si>
-    <t>"1112223334"</t>
-  </si>
-  <si>
-    <t>"60661"</t>
-  </si>
-  <si>
-    <t>United States</t>
+    <t>22</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>pripeee@priepp.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -264,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -272,9 +243,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="41" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -621,10 +596,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>11</v>
@@ -644,10 +619,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -658,8 +633,9 @@
     <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="6"/>
     <col min="9" max="9" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="13"/>
     <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.5" style="7" customWidth="1"/>
+    <col min="14" max="14" width="23.5" style="10" customWidth="1"/>
     <col min="15" max="15" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -686,7 +662,7 @@
         <v>14</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>15</v>
@@ -694,7 +670,7 @@
       <c r="J1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="11" t="s">
         <v>19</v>
       </c>
       <c r="L1" s="3" t="s">
@@ -703,7 +679,7 @@
       <c r="M1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="8" t="s">
         <v>21</v>
       </c>
       <c r="O1" s="3" t="s">
@@ -715,7 +691,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>24</v>
@@ -729,135 +705,135 @@
       <c r="E2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>51</v>
+      <c r="F2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="7">
+        <v>12</v>
+      </c>
+      <c r="H2" s="7">
+        <v>1985</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="12">
+        <v>60661</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="7">
+        <v>21</v>
+      </c>
+      <c r="N2" s="9">
+        <v>1112223334</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="P2" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="7">
+        <v>12</v>
+      </c>
+      <c r="H3" s="7">
+        <v>1985</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="12">
+        <v>60661</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="7">
+        <v>21</v>
+      </c>
+      <c r="N3" s="9">
+        <v>1112223334</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="P3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>53</v>
+      <c r="F4" s="7">
+        <v>8</v>
+      </c>
+      <c r="G4" s="7">
+        <v>6</v>
+      </c>
+      <c r="H4" s="7">
+        <v>1986</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="12">
+        <v>60661</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="7">
+        <v>21</v>
+      </c>
+      <c r="N4" s="9">
+        <v>1112223334</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>11</v>
@@ -865,13 +841,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>26</v>
@@ -879,35 +855,35 @@
       <c r="E5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>51</v>
+      <c r="F5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="7">
+        <v>8</v>
+      </c>
+      <c r="H5" s="7">
+        <v>2015</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="12">
+        <v>60661</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="7">
+        <v>21</v>
+      </c>
+      <c r="N5" s="9">
+        <v>1112223334</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>11</v>
@@ -915,13 +891,13 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>26</v>
@@ -929,47 +905,98 @@
       <c r="E6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>51</v>
+      <c r="F6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="7">
+        <v>7</v>
+      </c>
+      <c r="H6" s="7">
+        <v>1985</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="12">
+        <v>60661</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="7">
+        <v>21</v>
+      </c>
+      <c r="N6" s="9">
+        <v>1112223334</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N6" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="7">
+        <v>3</v>
+      </c>
+      <c r="H7" s="7">
+        <v>1985</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="12">
+        <v>60661</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" s="7">
+        <v>21</v>
+      </c>
+      <c r="N7" s="9">
+        <v>1112223334</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A6" r:id="rId4"/>
+    <hyperlink ref="A7" r:id="rId5"/>
+    <hyperlink ref="A2" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>